<commit_message>
Updates names and SQL
</commit_message>
<xml_diff>
--- a/L_registo_parcelas/LEGEND_L_registo_parcelas_cduats-media/LEGEND_L_registo_parcelas_cduats.xlsx
+++ b/L_registo_parcelas/LEGEND_L_registo_parcelas_cduats-media/LEGEND_L_registo_parcelas_cduats.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7380" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3295" uniqueCount="1557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3299" uniqueCount="1558">
   <si>
     <t>type</t>
   </si>
@@ -4755,14 +4755,24 @@
   <si>
     <t>Lembra se que a pessoa pode ser titular e representante ao mesmo tempo.</t>
   </si>
+  <si>
+    <t>Pessoa confirmada por testemunha</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -5021,363 +5031,363 @@
   </borders>
   <cellStyleXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="235" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="235" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="233" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="238" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="238" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="238" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="233" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="238" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="238" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="238" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5387,94 +5397,99 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="239">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6054,11 +6069,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P119"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="H105" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A107" sqref="A107"/>
+      <selection pane="bottomRight" activeCell="K70" sqref="K70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7295,6 +7310,9 @@
         <v>1317</v>
       </c>
       <c r="G70" s="76"/>
+      <c r="J70" s="104" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="71" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="74" t="s">
@@ -8014,13 +8032,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D169"/>
+  <dimension ref="A1:D170"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B146" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A161" sqref="A161:C163"/>
+      <selection pane="bottomRight" activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8824,28 +8842,28 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="20"/>
+      <c r="A81" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="B81" s="103" t="s">
+        <v>127</v>
+      </c>
+      <c r="C81" s="102" t="s">
+        <v>1557</v>
+      </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="63" t="s">
-        <v>259</v>
-      </c>
-      <c r="B82" s="22" t="s">
-        <v>254</v>
-      </c>
-      <c r="C82" s="12" t="s">
-        <v>247</v>
-      </c>
+      <c r="B82" s="20"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="63" t="s">
         <v>259</v>
       </c>
       <c r="B83" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -8853,10 +8871,10 @@
         <v>259</v>
       </c>
       <c r="B84" s="22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -8864,35 +8882,35 @@
         <v>259</v>
       </c>
       <c r="B85" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="63" t="s">
+        <v>259</v>
+      </c>
+      <c r="B86" s="22" t="s">
         <v>257</v>
       </c>
-      <c r="C85" s="12" t="s">
+      <c r="C86" s="12" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B86" s="20"/>
-    </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="B87" s="20" t="s">
-        <v>270</v>
-      </c>
-      <c r="C87" s="13" t="s">
-        <v>273</v>
-      </c>
+      <c r="B87" s="20"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>269</v>
       </c>
       <c r="B88" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -8900,10 +8918,10 @@
         <v>269</v>
       </c>
       <c r="B89" s="20" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -8911,62 +8929,62 @@
         <v>269</v>
       </c>
       <c r="B90" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="C90" s="13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B91" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="C90" s="13" t="s">
+      <c r="C91" s="13" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B91" s="20"/>
-    </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="B92" s="23" t="s">
-        <v>278</v>
-      </c>
-      <c r="C92" s="13" t="s">
-        <v>279</v>
-      </c>
+      <c r="B92" s="20"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="B93" s="38">
+      <c r="B93" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="C93" s="13" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B94" s="38">
         <v>1</v>
       </c>
-      <c r="C93" s="13" t="s">
+      <c r="C94" s="13" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="13"/>
-      <c r="B94" s="38"/>
-      <c r="C94" s="13"/>
-    </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="14" t="s">
-        <v>286</v>
-      </c>
-      <c r="B95" s="24" t="s">
-        <v>303</v>
-      </c>
-      <c r="C95" s="15" t="s">
-        <v>304</v>
-      </c>
+      <c r="A95" s="13"/>
+      <c r="B95" s="38"/>
+      <c r="C95" s="13"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
         <v>286</v>
       </c>
       <c r="B96" s="24" t="s">
-        <v>289</v>
+        <v>303</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>290</v>
+        <v>304</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -8974,10 +8992,10 @@
         <v>286</v>
       </c>
       <c r="B97" s="24" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -8985,10 +9003,10 @@
         <v>286</v>
       </c>
       <c r="B98" s="24" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -8996,10 +9014,10 @@
         <v>286</v>
       </c>
       <c r="B99" s="24" t="s">
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -9007,10 +9025,10 @@
         <v>286</v>
       </c>
       <c r="B100" s="24" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -9018,10 +9036,10 @@
         <v>286</v>
       </c>
       <c r="B101" s="24" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -9029,10 +9047,10 @@
         <v>286</v>
       </c>
       <c r="B102" s="24" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
       <c r="C102" s="15" t="s">
-        <v>294</v>
+        <v>306</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -9040,10 +9058,10 @@
         <v>286</v>
       </c>
       <c r="B103" s="24" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -9051,35 +9069,35 @@
         <v>286</v>
       </c>
       <c r="B104" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="C104" s="15" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="B105" s="24" t="s">
         <v>295</v>
       </c>
-      <c r="C104" s="25" t="s">
+      <c r="C105" s="25" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B105" s="20"/>
-    </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="26" t="s">
-        <v>217</v>
-      </c>
-      <c r="B106" s="66" t="s">
-        <v>218</v>
-      </c>
-      <c r="C106" s="26" t="s">
-        <v>219</v>
-      </c>
+      <c r="B106" s="20"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="26" t="s">
         <v>217</v>
       </c>
       <c r="B107" s="66" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C107" s="26" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -9087,10 +9105,10 @@
         <v>217</v>
       </c>
       <c r="B108" s="66" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C108" s="26" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -9098,10 +9116,10 @@
         <v>217</v>
       </c>
       <c r="B109" s="66" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C109" s="26" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -9109,10 +9127,10 @@
         <v>217</v>
       </c>
       <c r="B110" s="66" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C110" s="26" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -9120,10 +9138,10 @@
         <v>217</v>
       </c>
       <c r="B111" s="66" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C111" s="26" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -9131,10 +9149,10 @@
         <v>217</v>
       </c>
       <c r="B112" s="66" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C112" s="26" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -9142,10 +9160,10 @@
         <v>217</v>
       </c>
       <c r="B113" s="66" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C113" s="26" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -9153,10 +9171,10 @@
         <v>217</v>
       </c>
       <c r="B114" s="66" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C114" s="26" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -9164,10 +9182,10 @@
         <v>217</v>
       </c>
       <c r="B115" s="66" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C115" s="26" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -9175,64 +9193,64 @@
         <v>217</v>
       </c>
       <c r="B116" s="66" t="s">
+        <v>236</v>
+      </c>
+      <c r="C116" s="26" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="B117" s="66" t="s">
         <v>238</v>
       </c>
-      <c r="C116" s="26" t="s">
+      <c r="C117" s="26" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B117" s="67"/>
-    </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="B118" s="66" t="s">
-        <v>194</v>
-      </c>
-      <c r="C118" s="26" t="s">
-        <v>195</v>
-      </c>
+      <c r="B118" s="67"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="26" t="s">
         <v>193</v>
       </c>
       <c r="B119" s="66" t="s">
+        <v>194</v>
+      </c>
+      <c r="C119" s="26" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="B120" s="66" t="s">
         <v>196</v>
       </c>
-      <c r="C119" s="26" t="s">
+      <c r="C120" s="26" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="26"/>
-      <c r="B120" s="66" t="s">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="26"/>
+      <c r="B121" s="66" t="s">
         <v>198</v>
       </c>
-      <c r="C120" s="26"/>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="B121" s="66" t="s">
-        <v>200</v>
-      </c>
-      <c r="C121" s="26" t="s">
-        <v>201</v>
-      </c>
+      <c r="C121" s="26"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="26" t="s">
         <v>199</v>
       </c>
       <c r="B122" s="66" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C122" s="26" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -9240,37 +9258,37 @@
         <v>199</v>
       </c>
       <c r="B123" s="66" t="s">
+        <v>202</v>
+      </c>
+      <c r="C123" s="26" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="B124" s="66" t="s">
         <v>204</v>
       </c>
-      <c r="C123" s="26" t="s">
+      <c r="C124" s="26" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="26"/>
-      <c r="B124" s="27"/>
-      <c r="C124" s="26"/>
-    </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="26" t="s">
-        <v>206</v>
-      </c>
-      <c r="B125" s="66" t="s">
-        <v>207</v>
-      </c>
-      <c r="C125" s="26" t="s">
-        <v>208</v>
-      </c>
+      <c r="A125" s="26"/>
+      <c r="B125" s="27"/>
+      <c r="C125" s="26"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="26" t="s">
         <v>206</v>
       </c>
       <c r="B126" s="66" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C126" s="26" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -9278,10 +9296,10 @@
         <v>206</v>
       </c>
       <c r="B127" s="66" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C127" s="26" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -9289,10 +9307,10 @@
         <v>206</v>
       </c>
       <c r="B128" s="66" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C128" s="26" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -9300,37 +9318,37 @@
         <v>206</v>
       </c>
       <c r="B129" s="66" t="s">
+        <v>213</v>
+      </c>
+      <c r="C129" s="26" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="B130" s="66" t="s">
         <v>215</v>
       </c>
-      <c r="C129" s="26" t="s">
+      <c r="C130" s="26" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="26"/>
-      <c r="B130" s="27"/>
-      <c r="C130" s="26"/>
-    </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="26" t="s">
-        <v>1322</v>
-      </c>
-      <c r="B131" s="66" t="s">
-        <v>1323</v>
-      </c>
-      <c r="C131" s="26" t="s">
-        <v>1324</v>
-      </c>
+      <c r="A131" s="26"/>
+      <c r="B131" s="27"/>
+      <c r="C131" s="26"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="26" t="s">
         <v>1322</v>
       </c>
       <c r="B132" s="66" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="C132" s="26" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -9338,10 +9356,10 @@
         <v>1322</v>
       </c>
       <c r="B133" s="66" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="C133" s="26" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -9349,10 +9367,10 @@
         <v>1322</v>
       </c>
       <c r="B134" s="66" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="C134" s="26" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -9360,10 +9378,10 @@
         <v>1322</v>
       </c>
       <c r="B135" s="66" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="C135" s="26" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -9371,10 +9389,10 @@
         <v>1322</v>
       </c>
       <c r="B136" s="66" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="C136" s="26" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -9382,10 +9400,10 @@
         <v>1322</v>
       </c>
       <c r="B137" s="66" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="C137" s="26" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -9393,10 +9411,10 @@
         <v>1322</v>
       </c>
       <c r="B138" s="66" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="C138" s="26" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -9404,10 +9422,10 @@
         <v>1322</v>
       </c>
       <c r="B139" s="66" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="C139" s="26" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -9415,10 +9433,10 @@
         <v>1322</v>
       </c>
       <c r="B140" s="66" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="C140" s="26" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -9426,10 +9444,10 @@
         <v>1322</v>
       </c>
       <c r="B141" s="66" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="C141" s="26" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -9437,10 +9455,10 @@
         <v>1322</v>
       </c>
       <c r="B142" s="66" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="C142" s="26" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -9448,10 +9466,10 @@
         <v>1322</v>
       </c>
       <c r="B143" s="66" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="C143" s="26" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -9459,10 +9477,10 @@
         <v>1322</v>
       </c>
       <c r="B144" s="66" t="s">
-        <v>1322</v>
+        <v>1347</v>
       </c>
       <c r="C144" s="26" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -9470,10 +9488,10 @@
         <v>1322</v>
       </c>
       <c r="B145" s="66" t="s">
-        <v>1350</v>
+        <v>1322</v>
       </c>
       <c r="C145" s="26" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -9481,10 +9499,10 @@
         <v>1322</v>
       </c>
       <c r="B146" s="66" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="C146" s="26" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -9492,85 +9510,85 @@
         <v>1322</v>
       </c>
       <c r="B147" s="66" t="s">
+        <v>1352</v>
+      </c>
+      <c r="C147" s="26" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="26" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B148" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="C147" s="26" t="s">
+      <c r="C148" s="26" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B148" s="20"/>
-    </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="35" t="s">
-        <v>1426</v>
-      </c>
-      <c r="B149" s="36" t="s">
-        <v>1427</v>
-      </c>
-      <c r="C149" s="35" t="s">
-        <v>1428</v>
-      </c>
+      <c r="B149" s="20"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="35" t="s">
         <v>1426</v>
       </c>
       <c r="B150" s="36" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C150" s="35" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="35" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B151" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="C150" s="35" t="s">
+      <c r="C151" s="35" t="s">
         <v>1429</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B151" s="20"/>
-    </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" s="93" t="s">
+      <c r="B152" s="20"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="93" t="s">
         <v>1450</v>
       </c>
-      <c r="B152" s="94" t="s">
+      <c r="B153" s="94" t="s">
         <v>1446</v>
       </c>
-      <c r="C152" s="95" t="s">
+      <c r="C153" s="95" t="s">
         <v>1447</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" s="95" t="s">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="95" t="s">
         <v>1450</v>
       </c>
-      <c r="B153" s="94" t="s">
+      <c r="B154" s="94" t="s">
         <v>1448</v>
       </c>
-      <c r="C153" s="95" t="s">
+      <c r="C154" s="95" t="s">
         <v>1449</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B154" s="20"/>
-    </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="37" t="s">
-        <v>1451</v>
-      </c>
-      <c r="B155" s="65" t="s">
-        <v>1452</v>
-      </c>
-      <c r="C155" s="37" t="s">
-        <v>1453</v>
-      </c>
+      <c r="B155" s="20"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="37" t="s">
         <v>1451</v>
       </c>
       <c r="B156" s="65" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="C156" s="37" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -9578,10 +9596,10 @@
         <v>1451</v>
       </c>
       <c r="B157" s="65" t="s">
-        <v>136</v>
+        <v>1454</v>
       </c>
       <c r="C157" s="37" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -9589,46 +9607,46 @@
         <v>1451</v>
       </c>
       <c r="B158" s="65" t="s">
+        <v>136</v>
+      </c>
+      <c r="C158" s="37" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="37" t="s">
+        <v>1451</v>
+      </c>
+      <c r="B159" s="65" t="s">
         <v>1457</v>
       </c>
-      <c r="C158" s="63" t="s">
+      <c r="C159" s="63" t="s">
         <v>1486</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" s="63" t="s">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="63" t="s">
         <v>1451</v>
       </c>
-      <c r="B159" s="64" t="s">
+      <c r="B160" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="C159" s="63" t="s">
+      <c r="C160" s="63" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B160" s="20"/>
-    </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="92" t="s">
-        <v>1545</v>
-      </c>
-      <c r="B161" s="96" t="s">
-        <v>1549</v>
-      </c>
-      <c r="C161" s="92" t="s">
-        <v>1546</v>
-      </c>
+      <c r="B161" s="20"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="92" t="s">
         <v>1545</v>
       </c>
       <c r="B162" s="96" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="C162" s="92" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -9636,14 +9654,22 @@
         <v>1545</v>
       </c>
       <c r="B163" s="96" t="s">
+        <v>1550</v>
+      </c>
+      <c r="C163" s="92" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="92" t="s">
+        <v>1545</v>
+      </c>
+      <c r="B164" s="96" t="s">
         <v>1551</v>
       </c>
-      <c r="C163" s="92" t="s">
+      <c r="C164" s="92" t="s">
         <v>1548</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B164" s="20"/>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B165" s="20"/>
@@ -9659,6 +9685,9 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B169" s="20"/>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B170" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C18" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
@@ -34522,8 +34551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34557,7 +34586,7 @@
         <v>1499</v>
       </c>
       <c r="C2" s="99">
-        <v>201711131</v>
+        <v>201711151</v>
       </c>
       <c r="D2" s="101" t="s">
         <v>1401</v>

</xml_diff>

<commit_message>
Adds map geowidget to Form L, adds images for selection
</commit_message>
<xml_diff>
--- a/L_registo_parcelas/LEGEND_L_registo_parcelas_cduats-media/LEGEND_L_registo_parcelas_cduats.xlsx
+++ b/L_registo_parcelas/LEGEND_L_registo_parcelas_cduats-media/LEGEND_L_registo_parcelas_cduats.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3299" uniqueCount="1558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3305" uniqueCount="1562">
   <si>
     <t>type</t>
   </si>
@@ -4758,14 +4758,33 @@
   <si>
     <t>Pessoa confirmada por testemunha</t>
   </si>
+  <si>
+    <t>maps</t>
+  </si>
+  <si>
+    <t>Se a pessoa não estiver presente, escolha a imagem do dispositivo que mostra um rosto com uma cruz vermelha</t>
+  </si>
+  <si>
+    <t>Se a pessoa não tiver identificação com eles, escolha a imagem do dispositivo que mostra o cartão de identificação com uma cruz vermelha</t>
+  </si>
+  <si>
+    <t>Se a pessoa não estiver presente, não pode testemunhar</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -5031,363 +5050,363 @@
   </borders>
   <cellStyleXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="235" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="235" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="233" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="238" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="238" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="238" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="233" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="238" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="238" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="238" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5397,99 +5416,102 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="239">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6070,10 +6092,10 @@
   <dimension ref="A1:P119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H105" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E89" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K70" sqref="K70"/>
+      <selection pane="bottomRight" activeCell="F106" sqref="F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7295,6 +7317,9 @@
       <c r="C69" s="74" t="s">
         <v>1315</v>
       </c>
+      <c r="F69" s="106" t="s">
+        <v>1559</v>
+      </c>
       <c r="J69" s="97" t="s">
         <v>22</v>
       </c>
@@ -7309,6 +7334,9 @@
       <c r="C70" s="74" t="s">
         <v>1317</v>
       </c>
+      <c r="F70" s="106" t="s">
+        <v>1560</v>
+      </c>
       <c r="G70" s="76"/>
       <c r="J70" s="104" t="s">
         <v>22</v>
@@ -7857,6 +7885,9 @@
       <c r="C106" s="85" t="s">
         <v>1315</v>
       </c>
+      <c r="F106" s="107" t="s">
+        <v>1561</v>
+      </c>
       <c r="J106" s="98" t="s">
         <v>22</v>
       </c>
@@ -7870,6 +7901,9 @@
       </c>
       <c r="C107" s="85" t="s">
         <v>1317</v>
+      </c>
+      <c r="F107" s="107" t="s">
+        <v>1560</v>
       </c>
     </row>
     <row r="108" spans="1:12" s="85" customFormat="1" x14ac:dyDescent="0.25">
@@ -7930,6 +7964,9 @@
       <c r="J111" s="76" t="s">
         <v>22</v>
       </c>
+      <c r="L111" s="105" t="s">
+        <v>1558</v>
+      </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="74" t="s">
@@ -7972,6 +8009,9 @@
       <c r="D114" s="74"/>
       <c r="F114" s="74" t="s">
         <v>175</v>
+      </c>
+      <c r="L114" s="105" t="s">
+        <v>1558</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
@@ -34552,7 +34592,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34586,7 +34626,7 @@
         <v>1499</v>
       </c>
       <c r="C2" s="99">
-        <v>201711151</v>
+        <v>201711211</v>
       </c>
       <c r="D2" s="101" t="s">
         <v>1401</v>

</xml_diff>

<commit_message>
updates to form L
Spoke with simon re maps and names 27/11/17
</commit_message>
<xml_diff>
--- a/L_registo_parcelas/LEGEND_L_registo_parcelas_cduats-media/LEGEND_L_registo_parcelas_cduats.xlsx
+++ b/L_registo_parcelas/LEGEND_L_registo_parcelas_cduats-media/LEGEND_L_registo_parcelas_cduats.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3295" uniqueCount="1557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3297" uniqueCount="1558">
   <si>
     <t>type</t>
   </si>
@@ -4754,6 +4754,9 @@
   </si>
   <si>
     <t>Lembra se que a pessoa pode ser titular e representante ao mesmo tempo.</t>
+  </si>
+  <si>
+    <t>maps</t>
   </si>
 </sst>
 </file>
@@ -5260,7 +5263,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -5475,6 +5478,7 @@
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="239">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6055,10 +6059,10 @@
   <dimension ref="A1:P119"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C103" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A107" sqref="A107"/>
+      <selection pane="bottomRight" activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7912,6 +7916,9 @@
       <c r="J111" s="76" t="s">
         <v>22</v>
       </c>
+      <c r="L111" s="102" t="s">
+        <v>1557</v>
+      </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="74" t="s">
@@ -7954,6 +7961,9 @@
       <c r="D114" s="74"/>
       <c r="F114" s="74" t="s">
         <v>175</v>
+      </c>
+      <c r="L114" s="102" t="s">
+        <v>1557</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
@@ -34523,7 +34533,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34557,7 +34567,7 @@
         <v>1499</v>
       </c>
       <c r="C2" s="99">
-        <v>201711251</v>
+        <v>201711271</v>
       </c>
       <c r="D2" s="101" t="s">
         <v>1401</v>

</xml_diff>

<commit_message>
Updates to pessoas files
</commit_message>
<xml_diff>
--- a/L_registo_parcelas/LEGEND_L_registo_parcelas_cduats-media/LEGEND_L_registo_parcelas_cduats.xlsx
+++ b/L_registo_parcelas/LEGEND_L_registo_parcelas_cduats-media/LEGEND_L_registo_parcelas_cduats.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -4775,9 +4775,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -5050,363 +5057,363 @@
   </borders>
   <cellStyleXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="235" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="235" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="233" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="238" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="238" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="238" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="233" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="238" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="238" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="238" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5416,102 +5423,103 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="239">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -8075,10 +8083,10 @@
   <dimension ref="A1:D170"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B127" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D85" sqref="D85"/>
+      <selection pane="bottomRight" activeCell="F140" sqref="F140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9398,7 +9406,7 @@
       <c r="B133" s="66" t="s">
         <v>1325</v>
       </c>
-      <c r="C133" s="26" t="s">
+      <c r="C133" s="108" t="s">
         <v>1326</v>
       </c>
     </row>
@@ -9741,7 +9749,7 @@
   <dimension ref="A1:I4075"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A488" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A540" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D557" sqref="D557"/>
     </sheetView>
   </sheetViews>
@@ -34592,7 +34600,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34626,7 +34634,7 @@
         <v>1499</v>
       </c>
       <c r="C2" s="99">
-        <v>201801121</v>
+        <v>201802091</v>
       </c>
       <c r="D2" s="101" t="s">
         <v>1401</v>

</xml_diff>

<commit_message>
Fixes a bunch of things
</commit_message>
<xml_diff>
--- a/L_registo_parcelas/LEGEND_L_registo_parcelas_cduats-media/LEGEND_L_registo_parcelas_cduats.xlsx
+++ b/L_registo_parcelas/LEGEND_L_registo_parcelas_cduats-media/LEGEND_L_registo_parcelas_cduats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\legend\ODK Forms\legend-odk-forms\L_registo_parcelas\LEGEND_L_registo_parcelas_cduats-media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18461A7-E84A-4D50-8996-4E52FB12EE50}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBE5D29-37BC-40D3-85D3-2BCB0C7F3DD2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7380" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34601,7 +34601,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34635,7 +34635,7 @@
         <v>1499</v>
       </c>
       <c r="C2" s="99">
-        <v>201804021</v>
+        <v>201804201</v>
       </c>
       <c r="D2" s="101" t="s">
         <v>1401</v>

</xml_diff>

<commit_message>
Updates to LEGEND L and new Form O
</commit_message>
<xml_diff>
--- a/L_registo_parcelas/LEGEND_L_registo_parcelas_cduats-media/LEGEND_L_registo_parcelas_cduats.xlsx
+++ b/L_registo_parcelas/LEGEND_L_registo_parcelas_cduats-media/LEGEND_L_registo_parcelas_cduats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\legend\ODK Forms\legend-odk-forms\L_registo_parcelas\LEGEND_L_registo_parcelas_cduats-media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F850BA1B-2DBB-4D30-857E-AC05A6EE18DF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3277AEA1-5337-4130-B793-39260AD56ADF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7380" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35616,7 +35616,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35650,7 +35650,7 @@
         <v>1499</v>
       </c>
       <c r="C2" s="99">
-        <v>201808201</v>
+        <v>201808311</v>
       </c>
       <c r="D2" s="101" t="s">
         <v>1401</v>

</xml_diff>

<commit_message>
Updates to media for Form L
</commit_message>
<xml_diff>
--- a/L_registo_parcelas/LEGEND_L_registo_parcelas_cduats-media/LEGEND_L_registo_parcelas_cduats.xlsx
+++ b/L_registo_parcelas/LEGEND_L_registo_parcelas_cduats-media/LEGEND_L_registo_parcelas_cduats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\legend\ODK Forms\legend-odk-forms\L_registo_parcelas\LEGEND_L_registo_parcelas_cduats-media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3277AEA1-5337-4130-B793-39260AD56ADF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E619918-696A-4864-8E19-81F0C8DFBE22}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7380" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35616,7 +35616,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35650,7 +35650,7 @@
         <v>1499</v>
       </c>
       <c r="C2" s="99">
-        <v>201808311</v>
+        <v>201809201</v>
       </c>
       <c r="D2" s="101" t="s">
         <v>1401</v>

</xml_diff>